<commit_message>
changing the sheet name
</commit_message>
<xml_diff>
--- a/chat_log.xlsx
+++ b/chat_log.xlsx
@@ -7,8 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="test1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="test" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="test2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="test1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="test" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -461,7 +462,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>2024/08/06 19:46:41</t>
+          <t>2024/08/06 19:58:11</t>
         </is>
       </c>
     </row>
@@ -560,7 +561,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>2024/08/06 19:46:23</t>
+          <t>2024/08/06 19:46:41</t>
         </is>
       </c>
     </row>
@@ -636,4 +637,103 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="165" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>2024/08/06 19:46:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Role</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18" customHeight="1">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>Hello</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18" customHeight="1">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>assistant</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>AI assistant</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>how are you?</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="180" customHeight="1">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>assistant</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>I am fine
+ tha
+ nks,
+you?
+ not
+ much?
+ huh?
+ really?
+ how you doing
+ these days</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>